<commit_message>
Add the button to delete all candidats
</commit_message>
<xml_diff>
--- a/second_tour_website/website/upload/donees.xlsx
+++ b/second_tour_website/website/upload/donees.xlsx
@@ -432,1289 +432,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>id_creneau</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>id_candidat</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>id_matiere</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>id_salle</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>debut_preparation</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>fin</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>27</v>
-      </c>
-      <c r="D2" t="n">
-        <v>9</v>
-      </c>
-      <c r="E2" t="n">
-        <v>9</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>09:40</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="n">
-        <v>27</v>
-      </c>
-      <c r="D3" t="n">
-        <v>10</v>
-      </c>
-      <c r="E3" t="n">
-        <v>10</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>11:50</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" t="n">
-        <v>25</v>
-      </c>
-      <c r="D4" t="n">
-        <v>10</v>
-      </c>
-      <c r="E4" t="n">
-        <v>10</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>09:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>4</v>
-      </c>
-      <c r="C5" t="n">
-        <v>25</v>
-      </c>
-      <c r="D5" t="n">
-        <v>9</v>
-      </c>
-      <c r="E5" t="n">
-        <v>9</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>09:30</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>5</v>
-      </c>
-      <c r="C6" t="n">
-        <v>22</v>
-      </c>
-      <c r="D6" t="n">
-        <v>10</v>
-      </c>
-      <c r="E6" t="n">
-        <v>10</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>08:30</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>09:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>6</v>
-      </c>
-      <c r="C7" t="n">
-        <v>22</v>
-      </c>
-      <c r="D7" t="n">
-        <v>11</v>
-      </c>
-      <c r="E7" t="n">
-        <v>11</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>10:00</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>7</v>
-      </c>
-      <c r="C8" t="n">
-        <v>21</v>
-      </c>
-      <c r="D8" t="n">
-        <v>10</v>
-      </c>
-      <c r="E8" t="n">
-        <v>10</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>09:00</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>10:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>8</v>
-      </c>
-      <c r="C9" t="n">
-        <v>21</v>
-      </c>
-      <c r="D9" t="n">
-        <v>11</v>
-      </c>
-      <c r="E9" t="n">
-        <v>11</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>11:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>9</v>
-      </c>
-      <c r="C10" t="n">
-        <v>20</v>
-      </c>
-      <c r="D10" t="n">
-        <v>9</v>
-      </c>
-      <c r="E10" t="n">
-        <v>9</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>09:00</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>10</v>
-      </c>
-      <c r="C11" t="n">
-        <v>20</v>
-      </c>
-      <c r="D11" t="n">
-        <v>12</v>
-      </c>
-      <c r="E11" t="n">
-        <v>12</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
-        <v>11</v>
-      </c>
-      <c r="C12" t="n">
-        <v>19</v>
-      </c>
-      <c r="D12" t="n">
-        <v>9</v>
-      </c>
-      <c r="E12" t="n">
-        <v>9</v>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>10:00</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>11:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="n">
-        <v>12</v>
-      </c>
-      <c r="C13" t="n">
-        <v>19</v>
-      </c>
-      <c r="D13" t="n">
-        <v>10</v>
-      </c>
-      <c r="E13" t="n">
-        <v>10</v>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>13:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="n">
-        <v>13</v>
-      </c>
-      <c r="C14" t="n">
-        <v>18</v>
-      </c>
-      <c r="D14" t="n">
-        <v>9</v>
-      </c>
-      <c r="E14" t="n">
-        <v>9</v>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="n">
-        <v>14</v>
-      </c>
-      <c r="C15" t="n">
-        <v>17</v>
-      </c>
-      <c r="D15" t="n">
-        <v>9</v>
-      </c>
-      <c r="E15" t="n">
-        <v>9</v>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>12:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="n">
-        <v>15</v>
-      </c>
-      <c r="C16" t="n">
-        <v>17</v>
-      </c>
-      <c r="D16" t="n">
-        <v>10</v>
-      </c>
-      <c r="E16" t="n">
-        <v>10</v>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>09:30</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="n">
-        <v>16</v>
-      </c>
-      <c r="C17" t="n">
-        <v>16</v>
-      </c>
-      <c r="D17" t="n">
-        <v>9</v>
-      </c>
-      <c r="E17" t="n">
-        <v>9</v>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>11:30</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>13:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="n">
-        <v>17</v>
-      </c>
-      <c r="C18" t="n">
-        <v>15</v>
-      </c>
-      <c r="D18" t="n">
-        <v>9</v>
-      </c>
-      <c r="E18" t="n">
-        <v>9</v>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>14:00</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>15:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="n">
-        <v>18</v>
-      </c>
-      <c r="C19" t="n">
-        <v>15</v>
-      </c>
-      <c r="D19" t="n">
-        <v>10</v>
-      </c>
-      <c r="E19" t="n">
-        <v>10</v>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="n">
-        <v>19</v>
-      </c>
-      <c r="C20" t="n">
-        <v>7</v>
-      </c>
-      <c r="D20" t="n">
-        <v>9</v>
-      </c>
-      <c r="E20" t="n">
-        <v>9</v>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>14:30</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="n">
-        <v>20</v>
-      </c>
-      <c r="C21" t="n">
-        <v>7</v>
-      </c>
-      <c r="D21" t="n">
-        <v>11</v>
-      </c>
-      <c r="E21" t="n">
-        <v>11</v>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>16:30</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>17:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="n">
-        <v>21</v>
-      </c>
-      <c r="C22" t="n">
-        <v>6</v>
-      </c>
-      <c r="D22" t="n">
-        <v>9</v>
-      </c>
-      <c r="E22" t="n">
-        <v>9</v>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>15:00</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>16:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="n">
-        <v>22</v>
-      </c>
-      <c r="C23" t="n">
-        <v>6</v>
-      </c>
-      <c r="D23" t="n">
-        <v>10</v>
-      </c>
-      <c r="E23" t="n">
-        <v>10</v>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="n">
-        <v>23</v>
-      </c>
-      <c r="C24" t="n">
-        <v>4</v>
-      </c>
-      <c r="D24" t="n">
-        <v>9</v>
-      </c>
-      <c r="E24" t="n">
-        <v>9</v>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>15:30</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="n">
-        <v>24</v>
-      </c>
-      <c r="C25" t="n">
-        <v>4</v>
-      </c>
-      <c r="D25" t="n">
-        <v>10</v>
-      </c>
-      <c r="E25" t="n">
-        <v>10</v>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>14:00</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>15:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="n">
-        <v>25</v>
-      </c>
-      <c r="C26" t="n">
-        <v>3</v>
-      </c>
-      <c r="D26" t="n">
-        <v>5</v>
-      </c>
-      <c r="E26" t="n">
-        <v>7</v>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>09:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="n">
-        <v>26</v>
-      </c>
-      <c r="C27" t="n">
-        <v>3</v>
-      </c>
-      <c r="D27" t="n">
-        <v>6</v>
-      </c>
-      <c r="E27" t="n">
-        <v>8</v>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>09:30</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="n">
-        <v>27</v>
-      </c>
-      <c r="C28" t="n">
-        <v>8</v>
-      </c>
-      <c r="D28" t="n">
-        <v>1</v>
-      </c>
-      <c r="E28" t="n">
-        <v>3</v>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>09:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="n">
-        <v>28</v>
-      </c>
-      <c r="C29" t="n">
-        <v>8</v>
-      </c>
-      <c r="D29" t="n">
-        <v>3</v>
-      </c>
-      <c r="E29" t="n">
-        <v>5</v>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>09:30</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="n">
-        <v>29</v>
-      </c>
-      <c r="C30" t="n">
-        <v>9</v>
-      </c>
-      <c r="D30" t="n">
-        <v>2</v>
-      </c>
-      <c r="E30" t="n">
-        <v>4</v>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>09:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="n">
-        <v>30</v>
-      </c>
-      <c r="C31" t="n">
-        <v>9</v>
-      </c>
-      <c r="D31" t="n">
-        <v>3</v>
-      </c>
-      <c r="E31" t="n">
-        <v>5</v>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>10:00</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="n">
-        <v>31</v>
-      </c>
-      <c r="C32" t="n">
-        <v>10</v>
-      </c>
-      <c r="D32" t="n">
-        <v>1</v>
-      </c>
-      <c r="E32" t="n">
-        <v>3</v>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>08:30</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>09:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="n">
-        <v>32</v>
-      </c>
-      <c r="C33" t="n">
-        <v>10</v>
-      </c>
-      <c r="D33" t="n">
-        <v>2</v>
-      </c>
-      <c r="E33" t="n">
-        <v>4</v>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>10:00</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="n">
-        <v>33</v>
-      </c>
-      <c r="C34" t="n">
-        <v>11</v>
-      </c>
-      <c r="D34" t="n">
-        <v>5</v>
-      </c>
-      <c r="E34" t="n">
-        <v>7</v>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>08:30</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>09:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="n">
-        <v>34</v>
-      </c>
-      <c r="C35" t="n">
-        <v>11</v>
-      </c>
-      <c r="D35" t="n">
-        <v>6</v>
-      </c>
-      <c r="E35" t="n">
-        <v>8</v>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>10:00</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>11:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="n">
-        <v>35</v>
-      </c>
-      <c r="C36" t="n">
-        <v>12</v>
-      </c>
-      <c r="D36" t="n">
-        <v>5</v>
-      </c>
-      <c r="E36" t="n">
-        <v>7</v>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>09:00</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>10:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="n">
-        <v>36</v>
-      </c>
-      <c r="C37" t="n">
-        <v>12</v>
-      </c>
-      <c r="D37" t="n">
-        <v>6</v>
-      </c>
-      <c r="E37" t="n">
-        <v>8</v>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="n">
-        <v>37</v>
-      </c>
-      <c r="C38" t="n">
-        <v>13</v>
-      </c>
-      <c r="D38" t="n">
-        <v>5</v>
-      </c>
-      <c r="E38" t="n">
-        <v>7</v>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>09:30</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B39" t="n">
-        <v>38</v>
-      </c>
-      <c r="C39" t="n">
-        <v>13</v>
-      </c>
-      <c r="D39" t="n">
-        <v>6</v>
-      </c>
-      <c r="E39" t="n">
-        <v>8</v>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>12:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="B40" t="n">
-        <v>39</v>
-      </c>
-      <c r="C40" t="n">
-        <v>14</v>
-      </c>
-      <c r="D40" t="n">
-        <v>5</v>
-      </c>
-      <c r="E40" t="n">
-        <v>7</v>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>11:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="B41" t="n">
-        <v>40</v>
-      </c>
-      <c r="C41" t="n">
-        <v>14</v>
-      </c>
-      <c r="D41" t="n">
-        <v>7</v>
-      </c>
-      <c r="E41" t="n">
-        <v>5</v>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>09:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="B42" t="n">
-        <v>41</v>
-      </c>
-      <c r="C42" t="n">
-        <v>24</v>
-      </c>
-      <c r="D42" t="n">
-        <v>1</v>
-      </c>
-      <c r="E42" t="n">
-        <v>3</v>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>09:00</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>10:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="B43" t="n">
-        <v>42</v>
-      </c>
-      <c r="C43" t="n">
-        <v>24</v>
-      </c>
-      <c r="D43" t="n">
-        <v>3</v>
-      </c>
-      <c r="E43" t="n">
-        <v>5</v>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>11:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="B44" t="n">
-        <v>43</v>
-      </c>
-      <c r="C44" t="n">
-        <v>26</v>
-      </c>
-      <c r="D44" t="n">
-        <v>1</v>
-      </c>
-      <c r="E44" t="n">
-        <v>3</v>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>09:30</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B45" t="n">
-        <v>44</v>
-      </c>
-      <c r="C45" t="n">
-        <v>26</v>
-      </c>
-      <c r="D45" t="n">
-        <v>2</v>
-      </c>
-      <c r="E45" t="n">
-        <v>4</v>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="B46" t="n">
-        <v>45</v>
-      </c>
-      <c r="C46" t="n">
-        <v>16</v>
-      </c>
-      <c r="D46" t="n">
-        <v>10</v>
-      </c>
-      <c r="E46" t="n">
-        <v>10</v>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>10:00</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B47" t="n">
-        <v>46</v>
-      </c>
-      <c r="C47" t="n">
-        <v>18</v>
-      </c>
-      <c r="D47" t="n">
-        <v>10</v>
-      </c>
-      <c r="E47" t="n">
-        <v>10</v>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>14:30</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>15:30</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1765,23 +490,23 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Huon</t>
+          <t>Oumiri</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Guimond</t>
+          <t>Hakim</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -1789,23 +514,23 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Pinette</t>
+          <t>Garland</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Agathe</t>
+          <t>Gamelin</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1813,20 +538,20 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Jalbert</t>
+          <t>Huon</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Arienne</t>
+          <t>Guimond</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -1837,16 +562,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Bernard</t>
+          <t>Pinette</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Noémie</t>
+          <t>Agathe</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -1861,20 +586,20 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Gousse</t>
+          <t>Allain</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Maurice</t>
+          <t>Clothilde</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -1885,20 +610,20 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Le mendes</t>
+          <t>Jalbert</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Isaac</t>
+          <t>Arienne</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -1909,20 +634,20 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Guillot</t>
+          <t>Bernard</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Henri</t>
+          <t>Noémie</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -1933,20 +658,20 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Foucher</t>
+          <t>Gousse</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Maurice</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -1957,20 +682,20 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Duhamel</t>
+          <t>Le mendes</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Claire</t>
+          <t>Isaac</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -1981,20 +706,20 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Pons</t>
+          <t>Guillot</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Sebastien</t>
+          <t>Henri</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -2005,16 +730,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Vincent</t>
+          <t>Foucher</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Noémie</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -2029,20 +754,20 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Lefebvre</t>
+          <t>Duhamel</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Gilles</t>
+          <t>Claire</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -2053,20 +778,20 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Devaux</t>
+          <t>Pons</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Marine</t>
+          <t>Sebastien</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -2077,20 +802,20 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Labbe</t>
+          <t>Vincent</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Noémie</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -2101,16 +826,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Gomes</t>
+          <t>Lefebvre</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Aimé</t>
+          <t>Gilles</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -2125,16 +850,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Ribeiro</t>
+          <t>Devaux</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Alfred</t>
+          <t>Marine</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -2149,16 +874,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Romero</t>
+          <t>Labbe</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Julio</t>
+          <t>David</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -2173,16 +898,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Leroy</t>
+          <t>Gomes</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Benoît</t>
+          <t>Aimé</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -2197,16 +922,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Dias</t>
+          <t>Ribeiro</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Gilles</t>
+          <t>Alfred</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -2221,20 +946,20 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Garland</t>
+          <t>Romero</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Gamelin</t>
+          <t>Julio</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
@@ -2245,16 +970,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Lemaire</t>
+          <t>Leroy</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Alain</t>
+          <t>Benoît</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -2269,20 +994,20 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Oumiri</t>
+          <t>Dias</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Hakim</t>
+          <t>Gilles</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -2293,16 +1018,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Allain</t>
+          <t>Lemaire</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Clothilde</t>
+          <t>Alain</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -3531,16 +2256,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -3548,16 +2273,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -3565,16 +2290,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" t="n">
         <v>6</v>
-      </c>
-      <c r="C4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D4" t="n">
-        <v>9</v>
-      </c>
-      <c r="E4" t="n">
-        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -3582,16 +2307,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D5" t="n">
         <v>9</v>
       </c>
       <c r="E5" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -3599,16 +2324,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -3616,16 +2341,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" t="n">
         <v>9</v>
       </c>
-      <c r="C7" t="n">
-        <v>9</v>
-      </c>
-      <c r="D7" t="n">
-        <v>2</v>
-      </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -3633,16 +2358,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
@@ -3650,16 +2375,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -3667,16 +2392,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D10" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
@@ -3684,16 +2409,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -3701,16 +2426,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D12" t="n">
         <v>5</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
@@ -3718,16 +2443,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14">
@@ -3735,16 +2460,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15">
@@ -3752,16 +2477,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
@@ -3769,10 +2494,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D16" t="n">
         <v>9</v>
@@ -3786,10 +2511,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D17" t="n">
         <v>9</v>
@@ -3803,16 +2528,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D18" t="n">
         <v>9</v>
       </c>
       <c r="E18" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19">
@@ -3820,16 +2545,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D19" t="n">
+        <v>9</v>
+      </c>
+      <c r="E19" t="n">
         <v>10</v>
-      </c>
-      <c r="E19" t="n">
-        <v>11</v>
       </c>
     </row>
     <row r="20">
@@ -3837,16 +2562,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D20" t="n">
+        <v>9</v>
+      </c>
+      <c r="E20" t="n">
         <v>10</v>
-      </c>
-      <c r="E20" t="n">
-        <v>11</v>
       </c>
     </row>
     <row r="21">
@@ -3854,16 +2579,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22">
@@ -3871,16 +2596,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D22" t="n">
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23">
@@ -3888,16 +2613,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24">
@@ -3905,16 +2630,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D24" t="n">
+        <v>10</v>
+      </c>
+      <c r="E24" t="n">
         <v>9</v>
-      </c>
-      <c r="E24" t="n">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -3963,7 +2688,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -3972,7 +2697,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>b"\x17\xe9\x7f\x84}\x86\x10)\x02R\xc9\xea\xab\xfc\x9bu!\xbc{0`\x9f\x1c\x99\x9eT\x1b\xcbL\x01\xbd\xe0y\xee\xa9\xc3}\xab\xd7\x81\xae\\6\x9a\xecvIj'\xdb\xde\x1c\x1d\xefsPC\x02\xf4\xa5\x0b\x80%+"</t>
+          <t>b'\xf8\x9b!\x10\xc2\t\xefC\xef\xe5M\x14\xea\x08\x17\xe3\x82\x10\xbal\xb7\xad\x00\x83\x83\x88\x8f\x93\x88\xae\xef;\x81J`@\x04\x14\xa8+\x90\xbc]HBZ\\\xf2\xe3\xdf\xe9\xdb\xb7\xdcrB\x8d^\x80\xcc$A\xb9\xaf'</t>
         </is>
       </c>
       <c r="E2" t="b">
@@ -3984,16 +2709,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>prof@test.com</t>
+          <t>test@gmail.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>b"\x1a\xb0\xa2\xe7\xba\xf9g\x1a\x8b8^\xaa\xb5\x19\x1d\xef\xde9\xceo\xf3\x93F=\x07\x12\xa4\xd9teF\x82\xe1\x889\xb9\xa2\x9a\xa1\xb5\xdd\t\xd4\xfd1/\xdd3{\x96t\x191\xc6'\xa2\xb7\xd4(\xc3\xd5\xf2\x8b\xf7"</t>
+          <t>b'\xd6\x18\x00P\xc9\xeem\xc7\x11\xf2\x93\x99f\xde~0b\x9d\x8d\xca;\x1c\xe3\xaa\xd9c\\\x0c\xc0\x1e\x9f\xb1O^\x1e\xf1\x01}B][}\x97D6\xcf\x0f\xba\x85X~G\xa6C9\xe9\xb8\xf8\xce\xbf\xff\xb6\xb9I'</t>
         </is>
       </c>
       <c r="E3" t="b">

</xml_diff>